<commit_message>
Message sending is close, but IDK how close
Got it so that it should work but explodes instead
</commit_message>
<xml_diff>
--- a/Hours Spreadsheet Cutting Edge.xlsx
+++ b/Hours Spreadsheet Cutting Edge.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="35">
   <si>
     <t>Aaron's Hours Tracking</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>Got Server to spit out feed for messages, Can't get app to read the message</t>
+  </si>
+  <si>
+    <t>Tried to get messages working, but blew up the database</t>
+  </si>
+  <si>
+    <t>Got ass kicked by message code</t>
   </si>
 </sst>
 </file>
@@ -442,6 +448,9 @@
     <xf numFmtId="18" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -491,9 +500,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -800,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:D20"/>
+    <sheetView tabSelected="1" topLeftCell="J15" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22:Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -813,94 +819,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="25"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="27"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="28"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20" t="s">
+      <c r="F3" s="21"/>
+      <c r="G3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="29" t="s">
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="30"/>
-      <c r="L3" s="31"/>
-      <c r="M3" s="20" t="s">
+      <c r="K3" s="31"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="20" t="s">
+      <c r="N3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="22"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="21"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="22"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -1378,7 +1384,7 @@
         <v>0.55208333333333337</v>
       </c>
       <c r="F20" s="16"/>
-      <c r="G20" s="37">
+      <c r="G20" s="20">
         <v>0.11458333333333333</v>
       </c>
       <c r="H20" s="16"/>
@@ -1398,40 +1404,64 @@
       <c r="P20" s="17"/>
       <c r="Q20" s="18"/>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" s="6"/>
+    <row r="21" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="8"/>
+      <c r="E21" s="8">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="F21" s="7"/>
-      <c r="G21" s="8"/>
+      <c r="G21" s="8">
+        <v>0.66666666666666663</v>
+      </c>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
-      <c r="J21" s="7"/>
+      <c r="J21" s="7">
+        <v>2</v>
+      </c>
       <c r="K21" s="7"/>
       <c r="L21" s="7"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="9"/>
+      <c r="M21" s="4">
+        <v>42065</v>
+      </c>
+      <c r="N21" s="9" t="s">
+        <v>33</v>
+      </c>
       <c r="O21" s="9"/>
       <c r="P21" s="9"/>
       <c r="Q21" s="10"/>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
+    <row r="22" spans="1:17" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>17</v>
+      </c>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
-      <c r="E22" s="16"/>
+      <c r="E22" s="19">
+        <v>0.70833333333333337</v>
+      </c>
       <c r="F22" s="16"/>
-      <c r="G22" s="16"/>
+      <c r="G22" s="19">
+        <v>0.73958333333333337</v>
+      </c>
       <c r="H22" s="16"/>
       <c r="I22" s="16"/>
-      <c r="J22" s="16"/>
+      <c r="J22" s="16">
+        <v>0.75</v>
+      </c>
       <c r="K22" s="16"/>
       <c r="L22" s="16"/>
-      <c r="M22" s="3"/>
-      <c r="N22" s="17"/>
+      <c r="M22" s="5">
+        <v>42065</v>
+      </c>
+      <c r="N22" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="O22" s="17"/>
       <c r="P22" s="17"/>
       <c r="Q22" s="18"/>
@@ -2913,7 +2943,7 @@
       <c r="I100" s="12"/>
       <c r="J100" s="12">
         <f>SUM(J5:L99)</f>
-        <v>13.5</v>
+        <v>16.25</v>
       </c>
       <c r="K100" s="12"/>
       <c r="L100" s="12"/>
@@ -3432,94 +3462,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="25"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="27"/>
+      <c r="A2" s="26"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="28"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20" t="s">
+      <c r="F3" s="21"/>
+      <c r="G3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20" t="s">
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20" t="s">
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="N3" s="20" t="s">
+      <c r="N3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="22"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="21"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="22"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
@@ -5867,112 +5897,112 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="35"/>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35"/>
-      <c r="H2" s="35"/>
-      <c r="I2" s="35"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
+      <c r="G2" s="36"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35"/>
-      <c r="H3" s="35" t="s">
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36"/>
+      <c r="E3" s="36"/>
+      <c r="F3" s="36"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="35"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-      <c r="N3" s="35"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="36"/>
+      <c r="M3" s="36"/>
+      <c r="N3" s="36"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="36">
+      <c r="A5" s="37">
         <f>Sheet1!J100/(Sheet1!J100+Sheet2!J100)</f>
-        <v>0.98181818181818181</v>
-      </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
-      <c r="H5" s="36">
+        <v>0.98484848484848486</v>
+      </c>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
+      <c r="G5" s="37"/>
+      <c r="H5" s="37">
         <f>Sheet2!J100/(Sheet2!J100+Sheet1!J100)</f>
-        <v>1.8181818181818181E-2</v>
-      </c>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
-      <c r="K5" s="36"/>
-      <c r="L5" s="36"/>
-      <c r="M5" s="36"/>
-      <c r="N5" s="36"/>
+        <v>1.5151515151515152E-2</v>
+      </c>
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="37"/>
+      <c r="L5" s="37"/>
+      <c r="M5" s="37"/>
+      <c r="N5" s="37"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="36"/>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>